<commit_message>
se completa traslados y pedidos
Se realiza el ajuste de traslados, afecta los inventarios y se pueden cancelar, se completa la parte de pedidos, afecta inventarios
</commit_message>
<xml_diff>
--- a/Copias De Inventario.xlsx
+++ b/Copias De Inventario.xlsx
@@ -467,7 +467,7 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>1</v>
+        <v>695</v>
       </c>
       <c r="B2" t="n">
         <v>31</v>
@@ -488,12 +488,12 @@
         </is>
       </c>
       <c r="F2" t="n">
-        <v>53675</v>
+        <v>62894</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>2</v>
+        <v>696</v>
       </c>
       <c r="B3" t="n">
         <v>32</v>
@@ -514,12 +514,12 @@
         </is>
       </c>
       <c r="F3" t="n">
-        <v>3688</v>
+        <v>3691</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>3</v>
+        <v>697</v>
       </c>
       <c r="B4" t="n">
         <v>33</v>
@@ -540,12 +540,12 @@
         </is>
       </c>
       <c r="F4" t="n">
-        <v>3162</v>
+        <v>3165</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>4</v>
+        <v>698</v>
       </c>
       <c r="B5" t="n">
         <v>34</v>
@@ -566,12 +566,12 @@
         </is>
       </c>
       <c r="F5" t="n">
-        <v>31025</v>
+        <v>31370</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>5</v>
+        <v>699</v>
       </c>
       <c r="B6" t="n">
         <v>35</v>
@@ -592,12 +592,12 @@
         </is>
       </c>
       <c r="F6" t="n">
-        <v>25659</v>
+        <v>25779</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>6</v>
+        <v>700</v>
       </c>
       <c r="B7" t="n">
         <v>36</v>
@@ -618,12 +618,12 @@
         </is>
       </c>
       <c r="F7" t="n">
-        <v>46711</v>
+        <v>47302</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>7</v>
+        <v>701</v>
       </c>
       <c r="B8" t="n">
         <v>37</v>
@@ -644,12 +644,12 @@
         </is>
       </c>
       <c r="F8" t="n">
-        <v>12564</v>
+        <v>12702</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>8</v>
+        <v>702</v>
       </c>
       <c r="B9" t="n">
         <v>38</v>
@@ -670,12 +670,12 @@
         </is>
       </c>
       <c r="F9" t="n">
-        <v>-6</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>9</v>
+        <v>703</v>
       </c>
       <c r="B10" t="n">
         <v>41</v>
@@ -696,12 +696,12 @@
         </is>
       </c>
       <c r="F10" t="n">
-        <v>62846</v>
+        <v>63860</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>10</v>
+        <v>704</v>
       </c>
       <c r="B11" t="n">
         <v>42</v>
@@ -722,12 +722,12 @@
         </is>
       </c>
       <c r="F11" t="n">
-        <v>-3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>11</v>
+        <v>705</v>
       </c>
       <c r="B12" t="n">
         <v>43</v>
@@ -753,7 +753,7 @@
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>12</v>
+        <v>706</v>
       </c>
       <c r="B13" t="n">
         <v>44</v>
@@ -774,12 +774,12 @@
         </is>
       </c>
       <c r="F13" t="n">
-        <v>2276</v>
+        <v>2303</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>13</v>
+        <v>707</v>
       </c>
       <c r="B14" t="n">
         <v>45</v>
@@ -800,12 +800,12 @@
         </is>
       </c>
       <c r="F14" t="n">
-        <v>2810</v>
+        <v>2846</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>14</v>
+        <v>708</v>
       </c>
       <c r="B15" t="n">
         <v>46</v>
@@ -826,12 +826,12 @@
         </is>
       </c>
       <c r="F15" t="n">
-        <v>3057</v>
+        <v>3084</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>15</v>
+        <v>709</v>
       </c>
       <c r="B16" t="n">
         <v>47</v>
@@ -852,12 +852,12 @@
         </is>
       </c>
       <c r="F16" t="n">
-        <v>1194</v>
+        <v>1203</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>16</v>
+        <v>710</v>
       </c>
       <c r="B17" t="n">
         <v>48</v>
@@ -878,12 +878,12 @@
         </is>
       </c>
       <c r="F17" t="n">
-        <v>6869</v>
+        <v>6977</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>17</v>
+        <v>711</v>
       </c>
       <c r="B18" t="n">
         <v>49</v>
@@ -904,12 +904,12 @@
         </is>
       </c>
       <c r="F18" t="n">
-        <v>22006</v>
+        <v>22345</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>18</v>
+        <v>712</v>
       </c>
       <c r="B19" t="n">
         <v>410</v>
@@ -930,12 +930,12 @@
         </is>
       </c>
       <c r="F19" t="n">
-        <v>6011</v>
+        <v>6158</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>19</v>
+        <v>713</v>
       </c>
       <c r="B20" t="n">
         <v>411</v>
@@ -956,12 +956,12 @@
         </is>
       </c>
       <c r="F20" t="n">
-        <v>6866</v>
+        <v>6995</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>20</v>
+        <v>714</v>
       </c>
       <c r="B21" t="n">
         <v>412</v>
@@ -982,12 +982,12 @@
         </is>
       </c>
       <c r="F21" t="n">
-        <v>5018</v>
+        <v>5126</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="n">
-        <v>21</v>
+        <v>715</v>
       </c>
       <c r="B22" t="n">
         <v>51</v>
@@ -1008,12 +1008,12 @@
         </is>
       </c>
       <c r="F22" t="n">
-        <v>8256</v>
+        <v>8454</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="n">
-        <v>22</v>
+        <v>716</v>
       </c>
       <c r="B23" t="n">
         <v>52</v>
@@ -1034,12 +1034,12 @@
         </is>
       </c>
       <c r="F23" t="n">
-        <v>11137</v>
+        <v>11422</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="n">
-        <v>23</v>
+        <v>717</v>
       </c>
       <c r="B24" t="n">
         <v>53</v>
@@ -1060,12 +1060,12 @@
         </is>
       </c>
       <c r="F24" t="n">
-        <v>32369</v>
+        <v>32969</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="n">
-        <v>24</v>
+        <v>718</v>
       </c>
       <c r="B25" t="n">
         <v>54</v>
@@ -1086,12 +1086,12 @@
         </is>
       </c>
       <c r="F25" t="n">
-        <v>13027</v>
+        <v>13252</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="n">
-        <v>25</v>
+        <v>719</v>
       </c>
       <c r="B26" t="n">
         <v>55</v>
@@ -1112,12 +1112,12 @@
         </is>
       </c>
       <c r="F26" t="n">
-        <v>2059</v>
+        <v>2068</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="n">
-        <v>26</v>
+        <v>720</v>
       </c>
       <c r="B27" t="n">
         <v>56</v>
@@ -1143,7 +1143,7 @@
     </row>
     <row r="28">
       <c r="A28" t="n">
-        <v>27</v>
+        <v>721</v>
       </c>
       <c r="B28" t="n">
         <v>57</v>
@@ -1164,12 +1164,12 @@
         </is>
       </c>
       <c r="F28" t="n">
-        <v>3929</v>
+        <v>3971</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="n">
-        <v>28</v>
+        <v>722</v>
       </c>
       <c r="B29" t="n">
         <v>58</v>
@@ -1190,12 +1190,12 @@
         </is>
       </c>
       <c r="F29" t="n">
-        <v>17172</v>
+        <v>17451</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="n">
-        <v>29</v>
+        <v>723</v>
       </c>
       <c r="B30" t="n">
         <v>59</v>
@@ -1216,12 +1216,12 @@
         </is>
       </c>
       <c r="F30" t="n">
-        <v>40273</v>
+        <v>40804</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="n">
-        <v>30</v>
+        <v>724</v>
       </c>
       <c r="B31" t="n">
         <v>510</v>
@@ -1242,12 +1242,12 @@
         </is>
       </c>
       <c r="F31" t="n">
-        <v>5194</v>
+        <v>5296</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="n">
-        <v>31</v>
+        <v>725</v>
       </c>
       <c r="B32" t="n">
         <v>511</v>
@@ -1268,12 +1268,12 @@
         </is>
       </c>
       <c r="F32" t="n">
-        <v>890</v>
+        <v>905</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="n">
-        <v>32</v>
+        <v>726</v>
       </c>
       <c r="B33" t="n">
         <v>512</v>
@@ -1299,7 +1299,7 @@
     </row>
     <row r="34">
       <c r="A34" t="n">
-        <v>33</v>
+        <v>727</v>
       </c>
       <c r="B34" t="n">
         <v>513</v>
@@ -1325,7 +1325,7 @@
     </row>
     <row r="35">
       <c r="A35" t="n">
-        <v>34</v>
+        <v>728</v>
       </c>
       <c r="B35" t="n">
         <v>514</v>
@@ -1351,7 +1351,7 @@
     </row>
     <row r="36">
       <c r="A36" t="n">
-        <v>35</v>
+        <v>729</v>
       </c>
       <c r="B36" t="n">
         <v>515</v>
@@ -1377,7 +1377,7 @@
     </row>
     <row r="37">
       <c r="A37" t="n">
-        <v>36</v>
+        <v>730</v>
       </c>
       <c r="B37" t="n">
         <v>516</v>
@@ -1403,7 +1403,7 @@
     </row>
     <row r="38">
       <c r="A38" t="n">
-        <v>37</v>
+        <v>731</v>
       </c>
       <c r="B38" t="n">
         <v>517</v>
@@ -1429,7 +1429,7 @@
     </row>
     <row r="39">
       <c r="A39" t="n">
-        <v>38</v>
+        <v>732</v>
       </c>
       <c r="B39" t="n">
         <v>518</v>
@@ -1455,7 +1455,7 @@
     </row>
     <row r="40">
       <c r="A40" t="n">
-        <v>39</v>
+        <v>733</v>
       </c>
       <c r="B40" t="n">
         <v>519</v>
@@ -1481,7 +1481,7 @@
     </row>
     <row r="41">
       <c r="A41" t="n">
-        <v>40</v>
+        <v>734</v>
       </c>
       <c r="B41" t="n">
         <v>520</v>
@@ -1507,7 +1507,7 @@
     </row>
     <row r="42">
       <c r="A42" t="n">
-        <v>41</v>
+        <v>735</v>
       </c>
       <c r="B42" t="n">
         <v>521</v>
@@ -1533,7 +1533,7 @@
     </row>
     <row r="43">
       <c r="A43" t="n">
-        <v>42</v>
+        <v>736</v>
       </c>
       <c r="B43" t="n">
         <v>522</v>
@@ -1559,7 +1559,7 @@
     </row>
     <row r="44">
       <c r="A44" t="n">
-        <v>43</v>
+        <v>737</v>
       </c>
       <c r="B44" t="n">
         <v>523</v>
@@ -1585,7 +1585,7 @@
     </row>
     <row r="45">
       <c r="A45" t="n">
-        <v>44</v>
+        <v>738</v>
       </c>
       <c r="B45" t="n">
         <v>524</v>
@@ -1611,7 +1611,7 @@
     </row>
     <row r="46">
       <c r="A46" t="n">
-        <v>45</v>
+        <v>739</v>
       </c>
       <c r="B46" t="n">
         <v>1</v>
@@ -1637,7 +1637,7 @@
     </row>
     <row r="47">
       <c r="A47" t="n">
-        <v>46</v>
+        <v>740</v>
       </c>
       <c r="B47" t="n">
         <v>413</v>
@@ -1663,7 +1663,7 @@
     </row>
     <row r="48">
       <c r="A48" t="n">
-        <v>47</v>
+        <v>741</v>
       </c>
       <c r="B48" t="n">
         <v>414</v>
@@ -1689,7 +1689,7 @@
     </row>
     <row r="49">
       <c r="A49" t="n">
-        <v>48</v>
+        <v>742</v>
       </c>
       <c r="B49" t="n">
         <v>415</v>
@@ -1715,7 +1715,7 @@
     </row>
     <row r="50">
       <c r="A50" t="n">
-        <v>49</v>
+        <v>743</v>
       </c>
       <c r="B50" t="n">
         <v>416</v>
@@ -1741,7 +1741,7 @@
     </row>
     <row r="51">
       <c r="A51" t="n">
-        <v>50</v>
+        <v>744</v>
       </c>
       <c r="B51" t="n">
         <v>417</v>
@@ -1767,7 +1767,7 @@
     </row>
     <row r="52">
       <c r="A52" t="n">
-        <v>51</v>
+        <v>745</v>
       </c>
       <c r="B52" t="n">
         <v>418</v>
@@ -1793,7 +1793,7 @@
     </row>
     <row r="53">
       <c r="A53" t="n">
-        <v>52</v>
+        <v>746</v>
       </c>
       <c r="B53" t="n">
         <v>419</v>
@@ -1819,7 +1819,7 @@
     </row>
     <row r="54">
       <c r="A54" t="n">
-        <v>53</v>
+        <v>747</v>
       </c>
       <c r="B54" t="n">
         <v>420</v>
@@ -1845,7 +1845,7 @@
     </row>
     <row r="55">
       <c r="A55" t="n">
-        <v>54</v>
+        <v>748</v>
       </c>
       <c r="B55" t="n">
         <v>421</v>
@@ -1871,7 +1871,7 @@
     </row>
     <row r="56">
       <c r="A56" t="n">
-        <v>55</v>
+        <v>749</v>
       </c>
       <c r="B56" t="n">
         <v>2</v>
@@ -1897,7 +1897,7 @@
     </row>
     <row r="57">
       <c r="A57" t="n">
-        <v>56</v>
+        <v>750</v>
       </c>
       <c r="B57" t="n">
         <v>36</v>
@@ -1923,7 +1923,7 @@
     </row>
     <row r="58">
       <c r="A58" t="n">
-        <v>57</v>
+        <v>751</v>
       </c>
       <c r="B58" t="n">
         <v>41</v>
@@ -1949,7 +1949,7 @@
     </row>
     <row r="59">
       <c r="A59" t="n">
-        <v>58</v>
+        <v>752</v>
       </c>
       <c r="B59" t="n">
         <v>49</v>
@@ -1975,7 +1975,7 @@
     </row>
     <row r="60">
       <c r="A60" t="n">
-        <v>59</v>
+        <v>753</v>
       </c>
       <c r="B60" t="n">
         <v>53</v>
@@ -2001,7 +2001,7 @@
     </row>
     <row r="61">
       <c r="A61" t="n">
-        <v>60</v>
+        <v>754</v>
       </c>
       <c r="B61" t="n">
         <v>59</v>
@@ -2027,7 +2027,7 @@
     </row>
     <row r="62">
       <c r="A62" t="n">
-        <v>61</v>
+        <v>755</v>
       </c>
       <c r="B62" t="n">
         <v>512</v>
@@ -2053,7 +2053,7 @@
     </row>
     <row r="63">
       <c r="A63" t="n">
-        <v>62</v>
+        <v>756</v>
       </c>
       <c r="B63" t="n">
         <v>513</v>
@@ -2079,7 +2079,7 @@
     </row>
     <row r="64">
       <c r="A64" t="n">
-        <v>63</v>
+        <v>757</v>
       </c>
       <c r="B64" t="n">
         <v>514</v>
@@ -2105,7 +2105,7 @@
     </row>
     <row r="65">
       <c r="A65" t="n">
-        <v>64</v>
+        <v>758</v>
       </c>
       <c r="B65" t="n">
         <v>515</v>
@@ -2131,7 +2131,7 @@
     </row>
     <row r="66">
       <c r="A66" t="n">
-        <v>65</v>
+        <v>759</v>
       </c>
       <c r="B66" t="n">
         <v>516</v>
@@ -2157,7 +2157,7 @@
     </row>
     <row r="67">
       <c r="A67" t="n">
-        <v>66</v>
+        <v>760</v>
       </c>
       <c r="B67" t="n">
         <v>517</v>
@@ -2183,7 +2183,7 @@
     </row>
     <row r="68">
       <c r="A68" t="n">
-        <v>67</v>
+        <v>761</v>
       </c>
       <c r="B68" t="n">
         <v>518</v>
@@ -2209,7 +2209,7 @@
     </row>
     <row r="69">
       <c r="A69" t="n">
-        <v>68</v>
+        <v>762</v>
       </c>
       <c r="B69" t="n">
         <v>519</v>
@@ -2235,7 +2235,7 @@
     </row>
     <row r="70">
       <c r="A70" t="n">
-        <v>69</v>
+        <v>763</v>
       </c>
       <c r="B70" t="n">
         <v>520</v>
@@ -2261,7 +2261,7 @@
     </row>
     <row r="71">
       <c r="A71" t="n">
-        <v>70</v>
+        <v>764</v>
       </c>
       <c r="B71" t="n">
         <v>521</v>
@@ -2287,7 +2287,7 @@
     </row>
     <row r="72">
       <c r="A72" t="n">
-        <v>71</v>
+        <v>765</v>
       </c>
       <c r="B72" t="n">
         <v>522</v>
@@ -2313,7 +2313,7 @@
     </row>
     <row r="73">
       <c r="A73" t="n">
-        <v>72</v>
+        <v>766</v>
       </c>
       <c r="B73" t="n">
         <v>523</v>
@@ -2339,7 +2339,7 @@
     </row>
     <row r="74">
       <c r="A74" t="n">
-        <v>73</v>
+        <v>767</v>
       </c>
       <c r="B74" t="n">
         <v>31</v>
@@ -2360,12 +2360,12 @@
         </is>
       </c>
       <c r="F74" t="n">
-        <v>35967</v>
+        <v>36123</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="n">
-        <v>74</v>
+        <v>768</v>
       </c>
       <c r="B75" t="n">
         <v>32</v>
@@ -2391,7 +2391,7 @@
     </row>
     <row r="76">
       <c r="A76" t="n">
-        <v>75</v>
+        <v>769</v>
       </c>
       <c r="B76" t="n">
         <v>33</v>
@@ -2417,7 +2417,7 @@
     </row>
     <row r="77">
       <c r="A77" t="n">
-        <v>76</v>
+        <v>770</v>
       </c>
       <c r="B77" t="n">
         <v>34</v>
@@ -2438,12 +2438,12 @@
         </is>
       </c>
       <c r="F77" t="n">
-        <v>23631</v>
+        <v>23886</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="n">
-        <v>77</v>
+        <v>771</v>
       </c>
       <c r="B78" t="n">
         <v>35</v>
@@ -2464,12 +2464,12 @@
         </is>
       </c>
       <c r="F78" t="n">
-        <v>16264</v>
+        <v>16321</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="n">
-        <v>78</v>
+        <v>772</v>
       </c>
       <c r="B79" t="n">
         <v>36</v>
@@ -2490,12 +2490,12 @@
         </is>
       </c>
       <c r="F79" t="n">
-        <v>39742</v>
+        <v>40219</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="n">
-        <v>79</v>
+        <v>773</v>
       </c>
       <c r="B80" t="n">
         <v>37</v>
@@ -2516,12 +2516,12 @@
         </is>
       </c>
       <c r="F80" t="n">
-        <v>9259</v>
+        <v>9373</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="n">
-        <v>80</v>
+        <v>774</v>
       </c>
       <c r="B81" t="n">
         <v>38</v>
@@ -2547,7 +2547,7 @@
     </row>
     <row r="82">
       <c r="A82" t="n">
-        <v>81</v>
+        <v>775</v>
       </c>
       <c r="B82" t="n">
         <v>41</v>
@@ -2568,12 +2568,12 @@
         </is>
       </c>
       <c r="F82" t="n">
-        <v>50834</v>
+        <v>51593</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="n">
-        <v>82</v>
+        <v>776</v>
       </c>
       <c r="B83" t="n">
         <v>42</v>
@@ -2599,7 +2599,7 @@
     </row>
     <row r="84">
       <c r="A84" t="n">
-        <v>83</v>
+        <v>777</v>
       </c>
       <c r="B84" t="n">
         <v>43</v>
@@ -2625,7 +2625,7 @@
     </row>
     <row r="85">
       <c r="A85" t="n">
-        <v>84</v>
+        <v>778</v>
       </c>
       <c r="B85" t="n">
         <v>44</v>
@@ -2646,12 +2646,12 @@
         </is>
       </c>
       <c r="F85" t="n">
-        <v>900</v>
+        <v>909</v>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="n">
-        <v>85</v>
+        <v>779</v>
       </c>
       <c r="B86" t="n">
         <v>45</v>
@@ -2672,12 +2672,12 @@
         </is>
       </c>
       <c r="F86" t="n">
-        <v>1263</v>
+        <v>1281</v>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="n">
-        <v>86</v>
+        <v>780</v>
       </c>
       <c r="B87" t="n">
         <v>46</v>
@@ -2698,12 +2698,12 @@
         </is>
       </c>
       <c r="F87" t="n">
-        <v>1162</v>
+        <v>1177</v>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="n">
-        <v>87</v>
+        <v>781</v>
       </c>
       <c r="B88" t="n">
         <v>47</v>
@@ -2724,12 +2724,12 @@
         </is>
       </c>
       <c r="F88" t="n">
-        <v>700</v>
+        <v>712</v>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="n">
-        <v>88</v>
+        <v>782</v>
       </c>
       <c r="B89" t="n">
         <v>48</v>
@@ -2750,12 +2750,12 @@
         </is>
       </c>
       <c r="F89" t="n">
-        <v>3865</v>
+        <v>3925</v>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="n">
-        <v>89</v>
+        <v>783</v>
       </c>
       <c r="B90" t="n">
         <v>49</v>
@@ -2776,12 +2776,12 @@
         </is>
       </c>
       <c r="F90" t="n">
-        <v>18612</v>
+        <v>18882</v>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="n">
-        <v>90</v>
+        <v>784</v>
       </c>
       <c r="B91" t="n">
         <v>410</v>
@@ -2802,12 +2802,12 @@
         </is>
       </c>
       <c r="F91" t="n">
-        <v>5314</v>
+        <v>5455</v>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="n">
-        <v>91</v>
+        <v>785</v>
       </c>
       <c r="B92" t="n">
         <v>411</v>
@@ -2828,12 +2828,12 @@
         </is>
       </c>
       <c r="F92" t="n">
-        <v>5425</v>
+        <v>5506</v>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="n">
-        <v>92</v>
+        <v>786</v>
       </c>
       <c r="B93" t="n">
         <v>412</v>
@@ -2854,12 +2854,12 @@
         </is>
       </c>
       <c r="F93" t="n">
-        <v>3011</v>
+        <v>3062</v>
       </c>
     </row>
     <row r="94">
       <c r="A94" t="n">
-        <v>93</v>
+        <v>787</v>
       </c>
       <c r="B94" t="n">
         <v>51</v>
@@ -2880,12 +2880,12 @@
         </is>
       </c>
       <c r="F94" t="n">
-        <v>5370</v>
+        <v>5481</v>
       </c>
     </row>
     <row r="95">
       <c r="A95" t="n">
-        <v>94</v>
+        <v>788</v>
       </c>
       <c r="B95" t="n">
         <v>52</v>
@@ -2906,12 +2906,12 @@
         </is>
       </c>
       <c r="F95" t="n">
-        <v>12728</v>
+        <v>13076</v>
       </c>
     </row>
     <row r="96">
       <c r="A96" t="n">
-        <v>95</v>
+        <v>789</v>
       </c>
       <c r="B96" t="n">
         <v>53</v>
@@ -2932,12 +2932,12 @@
         </is>
       </c>
       <c r="F96" t="n">
-        <v>29013</v>
+        <v>29643</v>
       </c>
     </row>
     <row r="97">
       <c r="A97" t="n">
-        <v>96</v>
+        <v>790</v>
       </c>
       <c r="B97" t="n">
         <v>54</v>
@@ -2958,12 +2958,12 @@
         </is>
       </c>
       <c r="F97" t="n">
-        <v>11409</v>
+        <v>11601</v>
       </c>
     </row>
     <row r="98">
       <c r="A98" t="n">
-        <v>97</v>
+        <v>791</v>
       </c>
       <c r="B98" t="n">
         <v>55</v>
@@ -2984,12 +2984,12 @@
         </is>
       </c>
       <c r="F98" t="n">
-        <v>1836</v>
+        <v>1851</v>
       </c>
     </row>
     <row r="99">
       <c r="A99" t="n">
-        <v>98</v>
+        <v>792</v>
       </c>
       <c r="B99" t="n">
         <v>56</v>
@@ -3015,7 +3015,7 @@
     </row>
     <row r="100">
       <c r="A100" t="n">
-        <v>99</v>
+        <v>793</v>
       </c>
       <c r="B100" t="n">
         <v>57</v>
@@ -3036,12 +3036,12 @@
         </is>
       </c>
       <c r="F100" t="n">
-        <v>3021</v>
+        <v>3036</v>
       </c>
     </row>
     <row r="101">
       <c r="A101" t="n">
-        <v>100</v>
+        <v>794</v>
       </c>
       <c r="B101" t="n">
         <v>58</v>
@@ -3062,12 +3062,12 @@
         </is>
       </c>
       <c r="F101" t="n">
-        <v>10541</v>
+        <v>10739</v>
       </c>
     </row>
     <row r="102">
       <c r="A102" t="n">
-        <v>101</v>
+        <v>795</v>
       </c>
       <c r="B102" t="n">
         <v>59</v>
@@ -3088,12 +3088,12 @@
         </is>
       </c>
       <c r="F102" t="n">
-        <v>37613</v>
+        <v>38129</v>
       </c>
     </row>
     <row r="103">
       <c r="A103" t="n">
-        <v>102</v>
+        <v>796</v>
       </c>
       <c r="B103" t="n">
         <v>510</v>
@@ -3114,12 +3114,12 @@
         </is>
       </c>
       <c r="F103" t="n">
-        <v>5042</v>
+        <v>5153</v>
       </c>
     </row>
     <row r="104">
       <c r="A104" t="n">
-        <v>103</v>
+        <v>797</v>
       </c>
       <c r="B104" t="n">
         <v>511</v>
@@ -3140,12 +3140,12 @@
         </is>
       </c>
       <c r="F104" t="n">
-        <v>566</v>
+        <v>569</v>
       </c>
     </row>
     <row r="105">
       <c r="A105" t="n">
-        <v>104</v>
+        <v>798</v>
       </c>
       <c r="B105" t="n">
         <v>512</v>
@@ -3171,7 +3171,7 @@
     </row>
     <row r="106">
       <c r="A106" t="n">
-        <v>105</v>
+        <v>799</v>
       </c>
       <c r="B106" t="n">
         <v>513</v>
@@ -3197,7 +3197,7 @@
     </row>
     <row r="107">
       <c r="A107" t="n">
-        <v>106</v>
+        <v>800</v>
       </c>
       <c r="B107" t="n">
         <v>514</v>
@@ -3223,7 +3223,7 @@
     </row>
     <row r="108">
       <c r="A108" t="n">
-        <v>107</v>
+        <v>801</v>
       </c>
       <c r="B108" t="n">
         <v>515</v>
@@ -3249,7 +3249,7 @@
     </row>
     <row r="109">
       <c r="A109" t="n">
-        <v>108</v>
+        <v>802</v>
       </c>
       <c r="B109" t="n">
         <v>516</v>
@@ -3275,7 +3275,7 @@
     </row>
     <row r="110">
       <c r="A110" t="n">
-        <v>109</v>
+        <v>803</v>
       </c>
       <c r="B110" t="n">
         <v>517</v>
@@ -3301,7 +3301,7 @@
     </row>
     <row r="111">
       <c r="A111" t="n">
-        <v>110</v>
+        <v>804</v>
       </c>
       <c r="B111" t="n">
         <v>518</v>
@@ -3327,7 +3327,7 @@
     </row>
     <row r="112">
       <c r="A112" t="n">
-        <v>111</v>
+        <v>805</v>
       </c>
       <c r="B112" t="n">
         <v>519</v>
@@ -3353,7 +3353,7 @@
     </row>
     <row r="113">
       <c r="A113" t="n">
-        <v>112</v>
+        <v>806</v>
       </c>
       <c r="B113" t="n">
         <v>520</v>
@@ -3379,7 +3379,7 @@
     </row>
     <row r="114">
       <c r="A114" t="n">
-        <v>113</v>
+        <v>807</v>
       </c>
       <c r="B114" t="n">
         <v>521</v>
@@ -3405,7 +3405,7 @@
     </row>
     <row r="115">
       <c r="A115" t="n">
-        <v>114</v>
+        <v>808</v>
       </c>
       <c r="B115" t="n">
         <v>522</v>
@@ -3431,7 +3431,7 @@
     </row>
     <row r="116">
       <c r="A116" t="n">
-        <v>115</v>
+        <v>809</v>
       </c>
       <c r="B116" t="n">
         <v>523</v>
@@ -3457,7 +3457,7 @@
     </row>
     <row r="117">
       <c r="A117" t="n">
-        <v>116</v>
+        <v>810</v>
       </c>
       <c r="B117" t="n">
         <v>524</v>
@@ -3483,7 +3483,7 @@
     </row>
     <row r="118">
       <c r="A118" t="n">
-        <v>117</v>
+        <v>811</v>
       </c>
       <c r="B118" t="n">
         <v>1</v>
@@ -3509,7 +3509,7 @@
     </row>
     <row r="119">
       <c r="A119" t="n">
-        <v>118</v>
+        <v>812</v>
       </c>
       <c r="B119" t="n">
         <v>413</v>
@@ -3535,7 +3535,7 @@
     </row>
     <row r="120">
       <c r="A120" t="n">
-        <v>119</v>
+        <v>813</v>
       </c>
       <c r="B120" t="n">
         <v>414</v>
@@ -3561,7 +3561,7 @@
     </row>
     <row r="121">
       <c r="A121" t="n">
-        <v>120</v>
+        <v>814</v>
       </c>
       <c r="B121" t="n">
         <v>415</v>
@@ -3587,7 +3587,7 @@
     </row>
     <row r="122">
       <c r="A122" t="n">
-        <v>121</v>
+        <v>815</v>
       </c>
       <c r="B122" t="n">
         <v>416</v>
@@ -3613,7 +3613,7 @@
     </row>
     <row r="123">
       <c r="A123" t="n">
-        <v>122</v>
+        <v>816</v>
       </c>
       <c r="B123" t="n">
         <v>417</v>
@@ -3639,7 +3639,7 @@
     </row>
     <row r="124">
       <c r="A124" t="n">
-        <v>123</v>
+        <v>817</v>
       </c>
       <c r="B124" t="n">
         <v>418</v>
@@ -3665,7 +3665,7 @@
     </row>
     <row r="125">
       <c r="A125" t="n">
-        <v>124</v>
+        <v>818</v>
       </c>
       <c r="B125" t="n">
         <v>419</v>
@@ -3691,7 +3691,7 @@
     </row>
     <row r="126">
       <c r="A126" t="n">
-        <v>125</v>
+        <v>819</v>
       </c>
       <c r="B126" t="n">
         <v>420</v>
@@ -3717,7 +3717,7 @@
     </row>
     <row r="127">
       <c r="A127" t="n">
-        <v>126</v>
+        <v>820</v>
       </c>
       <c r="B127" t="n">
         <v>421</v>
@@ -3743,7 +3743,7 @@
     </row>
     <row r="128">
       <c r="A128" t="n">
-        <v>127</v>
+        <v>821</v>
       </c>
       <c r="B128" t="n">
         <v>2</v>
@@ -3769,7 +3769,7 @@
     </row>
     <row r="129">
       <c r="A129" t="n">
-        <v>128</v>
+        <v>822</v>
       </c>
       <c r="B129" t="n">
         <v>31</v>
@@ -3790,12 +3790,12 @@
         </is>
       </c>
       <c r="F129" t="n">
-        <v>15817</v>
+        <v>16886</v>
       </c>
     </row>
     <row r="130">
       <c r="A130" t="n">
-        <v>129</v>
+        <v>823</v>
       </c>
       <c r="B130" t="n">
         <v>32</v>
@@ -3821,7 +3821,7 @@
     </row>
     <row r="131">
       <c r="A131" t="n">
-        <v>130</v>
+        <v>824</v>
       </c>
       <c r="B131" t="n">
         <v>33</v>
@@ -3847,7 +3847,7 @@
     </row>
     <row r="132">
       <c r="A132" t="n">
-        <v>131</v>
+        <v>825</v>
       </c>
       <c r="B132" t="n">
         <v>34</v>
@@ -3868,12 +3868,12 @@
         </is>
       </c>
       <c r="F132" t="n">
-        <v>8050</v>
+        <v>8125</v>
       </c>
     </row>
     <row r="133">
       <c r="A133" t="n">
-        <v>132</v>
+        <v>826</v>
       </c>
       <c r="B133" t="n">
         <v>35</v>
@@ -3894,12 +3894,12 @@
         </is>
       </c>
       <c r="F133" t="n">
-        <v>6282</v>
+        <v>6318</v>
       </c>
     </row>
     <row r="134">
       <c r="A134" t="n">
-        <v>133</v>
+        <v>827</v>
       </c>
       <c r="B134" t="n">
         <v>36</v>
@@ -3920,12 +3920,12 @@
         </is>
       </c>
       <c r="F134" t="n">
-        <v>15771</v>
+        <v>15975</v>
       </c>
     </row>
     <row r="135">
       <c r="A135" t="n">
-        <v>134</v>
+        <v>828</v>
       </c>
       <c r="B135" t="n">
         <v>37</v>
@@ -3946,12 +3946,12 @@
         </is>
       </c>
       <c r="F135" t="n">
-        <v>2926</v>
+        <v>2938</v>
       </c>
     </row>
     <row r="136">
       <c r="A136" t="n">
-        <v>135</v>
+        <v>829</v>
       </c>
       <c r="B136" t="n">
         <v>38</v>
@@ -3977,7 +3977,7 @@
     </row>
     <row r="137">
       <c r="A137" t="n">
-        <v>136</v>
+        <v>830</v>
       </c>
       <c r="B137" t="n">
         <v>41</v>
@@ -3998,12 +3998,12 @@
         </is>
       </c>
       <c r="F137" t="n">
-        <v>21262</v>
+        <v>21502</v>
       </c>
     </row>
     <row r="138">
       <c r="A138" t="n">
-        <v>137</v>
+        <v>831</v>
       </c>
       <c r="B138" t="n">
         <v>42</v>
@@ -4029,7 +4029,7 @@
     </row>
     <row r="139">
       <c r="A139" t="n">
-        <v>138</v>
+        <v>832</v>
       </c>
       <c r="B139" t="n">
         <v>43</v>
@@ -4055,7 +4055,7 @@
     </row>
     <row r="140">
       <c r="A140" t="n">
-        <v>139</v>
+        <v>833</v>
       </c>
       <c r="B140" t="n">
         <v>44</v>
@@ -4081,7 +4081,7 @@
     </row>
     <row r="141">
       <c r="A141" t="n">
-        <v>140</v>
+        <v>834</v>
       </c>
       <c r="B141" t="n">
         <v>45</v>
@@ -4102,12 +4102,12 @@
         </is>
       </c>
       <c r="F141" t="n">
-        <v>786</v>
+        <v>789</v>
       </c>
     </row>
     <row r="142">
       <c r="A142" t="n">
-        <v>141</v>
+        <v>835</v>
       </c>
       <c r="B142" t="n">
         <v>46</v>
@@ -4128,12 +4128,12 @@
         </is>
       </c>
       <c r="F142" t="n">
-        <v>603</v>
+        <v>612</v>
       </c>
     </row>
     <row r="143">
       <c r="A143" t="n">
-        <v>142</v>
+        <v>836</v>
       </c>
       <c r="B143" t="n">
         <v>47</v>
@@ -4154,12 +4154,12 @@
         </is>
       </c>
       <c r="F143" t="n">
-        <v>319</v>
+        <v>325</v>
       </c>
     </row>
     <row r="144">
       <c r="A144" t="n">
-        <v>143</v>
+        <v>837</v>
       </c>
       <c r="B144" t="n">
         <v>48</v>
@@ -4180,12 +4180,12 @@
         </is>
       </c>
       <c r="F144" t="n">
-        <v>1411</v>
+        <v>1417</v>
       </c>
     </row>
     <row r="145">
       <c r="A145" t="n">
-        <v>144</v>
+        <v>838</v>
       </c>
       <c r="B145" t="n">
         <v>49</v>
@@ -4206,12 +4206,12 @@
         </is>
       </c>
       <c r="F145" t="n">
-        <v>6019</v>
+        <v>6079</v>
       </c>
     </row>
     <row r="146">
       <c r="A146" t="n">
-        <v>145</v>
+        <v>839</v>
       </c>
       <c r="B146" t="n">
         <v>410</v>
@@ -4232,12 +4232,12 @@
         </is>
       </c>
       <c r="F146" t="n">
-        <v>1209</v>
+        <v>1230</v>
       </c>
     </row>
     <row r="147">
       <c r="A147" t="n">
-        <v>146</v>
+        <v>840</v>
       </c>
       <c r="B147" t="n">
         <v>411</v>
@@ -4258,12 +4258,12 @@
         </is>
       </c>
       <c r="F147" t="n">
-        <v>1390</v>
+        <v>1408</v>
       </c>
     </row>
     <row r="148">
       <c r="A148" t="n">
-        <v>147</v>
+        <v>841</v>
       </c>
       <c r="B148" t="n">
         <v>412</v>
@@ -4284,12 +4284,12 @@
         </is>
       </c>
       <c r="F148" t="n">
-        <v>1404</v>
+        <v>1422</v>
       </c>
     </row>
     <row r="149">
       <c r="A149" t="n">
-        <v>148</v>
+        <v>842</v>
       </c>
       <c r="B149" t="n">
         <v>51</v>
@@ -4310,12 +4310,12 @@
         </is>
       </c>
       <c r="F149" t="n">
-        <v>2720</v>
+        <v>2765</v>
       </c>
     </row>
     <row r="150">
       <c r="A150" t="n">
-        <v>149</v>
+        <v>843</v>
       </c>
       <c r="B150" t="n">
         <v>52</v>
@@ -4336,12 +4336,12 @@
         </is>
       </c>
       <c r="F150" t="n">
-        <v>2414</v>
+        <v>2471</v>
       </c>
     </row>
     <row r="151">
       <c r="A151" t="n">
-        <v>150</v>
+        <v>844</v>
       </c>
       <c r="B151" t="n">
         <v>53</v>
@@ -4362,12 +4362,12 @@
         </is>
       </c>
       <c r="F151" t="n">
-        <v>11094</v>
+        <v>11295</v>
       </c>
     </row>
     <row r="152">
       <c r="A152" t="n">
-        <v>151</v>
+        <v>845</v>
       </c>
       <c r="B152" t="n">
         <v>54</v>
@@ -4388,12 +4388,12 @@
         </is>
       </c>
       <c r="F152" t="n">
-        <v>4599</v>
+        <v>4692</v>
       </c>
     </row>
     <row r="153">
       <c r="A153" t="n">
-        <v>152</v>
+        <v>846</v>
       </c>
       <c r="B153" t="n">
         <v>55</v>
@@ -4414,12 +4414,12 @@
         </is>
       </c>
       <c r="F153" t="n">
-        <v>555</v>
+        <v>558</v>
       </c>
     </row>
     <row r="154">
       <c r="A154" t="n">
-        <v>153</v>
+        <v>847</v>
       </c>
       <c r="B154" t="n">
         <v>56</v>
@@ -4445,7 +4445,7 @@
     </row>
     <row r="155">
       <c r="A155" t="n">
-        <v>154</v>
+        <v>848</v>
       </c>
       <c r="B155" t="n">
         <v>57</v>
@@ -4466,12 +4466,12 @@
         </is>
       </c>
       <c r="F155" t="n">
-        <v>1476</v>
+        <v>1488</v>
       </c>
     </row>
     <row r="156">
       <c r="A156" t="n">
-        <v>155</v>
+        <v>849</v>
       </c>
       <c r="B156" t="n">
         <v>58</v>
@@ -4492,12 +4492,12 @@
         </is>
       </c>
       <c r="F156" t="n">
-        <v>4184</v>
+        <v>4262</v>
       </c>
     </row>
     <row r="157">
       <c r="A157" t="n">
-        <v>156</v>
+        <v>850</v>
       </c>
       <c r="B157" t="n">
         <v>59</v>
@@ -4518,12 +4518,12 @@
         </is>
       </c>
       <c r="F157" t="n">
-        <v>12345</v>
+        <v>12483</v>
       </c>
     </row>
     <row r="158">
       <c r="A158" t="n">
-        <v>157</v>
+        <v>851</v>
       </c>
       <c r="B158" t="n">
         <v>510</v>
@@ -4544,12 +4544,12 @@
         </is>
       </c>
       <c r="F158" t="n">
-        <v>1273</v>
+        <v>1297</v>
       </c>
     </row>
     <row r="159">
       <c r="A159" t="n">
-        <v>158</v>
+        <v>852</v>
       </c>
       <c r="B159" t="n">
         <v>511</v>
@@ -4570,12 +4570,12 @@
         </is>
       </c>
       <c r="F159" t="n">
-        <v>285</v>
+        <v>288</v>
       </c>
     </row>
     <row r="160">
       <c r="A160" t="n">
-        <v>159</v>
+        <v>853</v>
       </c>
       <c r="B160" t="n">
         <v>512</v>
@@ -4601,7 +4601,7 @@
     </row>
     <row r="161">
       <c r="A161" t="n">
-        <v>160</v>
+        <v>854</v>
       </c>
       <c r="B161" t="n">
         <v>513</v>
@@ -4627,7 +4627,7 @@
     </row>
     <row r="162">
       <c r="A162" t="n">
-        <v>161</v>
+        <v>855</v>
       </c>
       <c r="B162" t="n">
         <v>514</v>
@@ -4653,7 +4653,7 @@
     </row>
     <row r="163">
       <c r="A163" t="n">
-        <v>162</v>
+        <v>856</v>
       </c>
       <c r="B163" t="n">
         <v>515</v>
@@ -4679,7 +4679,7 @@
     </row>
     <row r="164">
       <c r="A164" t="n">
-        <v>163</v>
+        <v>857</v>
       </c>
       <c r="B164" t="n">
         <v>516</v>
@@ -4705,7 +4705,7 @@
     </row>
     <row r="165">
       <c r="A165" t="n">
-        <v>164</v>
+        <v>858</v>
       </c>
       <c r="B165" t="n">
         <v>517</v>
@@ -4731,7 +4731,7 @@
     </row>
     <row r="166">
       <c r="A166" t="n">
-        <v>165</v>
+        <v>859</v>
       </c>
       <c r="B166" t="n">
         <v>518</v>
@@ -4757,7 +4757,7 @@
     </row>
     <row r="167">
       <c r="A167" t="n">
-        <v>166</v>
+        <v>860</v>
       </c>
       <c r="B167" t="n">
         <v>519</v>
@@ -4783,7 +4783,7 @@
     </row>
     <row r="168">
       <c r="A168" t="n">
-        <v>167</v>
+        <v>861</v>
       </c>
       <c r="B168" t="n">
         <v>520</v>
@@ -4809,7 +4809,7 @@
     </row>
     <row r="169">
       <c r="A169" t="n">
-        <v>168</v>
+        <v>862</v>
       </c>
       <c r="B169" t="n">
         <v>521</v>
@@ -4835,7 +4835,7 @@
     </row>
     <row r="170">
       <c r="A170" t="n">
-        <v>169</v>
+        <v>863</v>
       </c>
       <c r="B170" t="n">
         <v>522</v>
@@ -4861,7 +4861,7 @@
     </row>
     <row r="171">
       <c r="A171" t="n">
-        <v>170</v>
+        <v>864</v>
       </c>
       <c r="B171" t="n">
         <v>523</v>
@@ -4887,7 +4887,7 @@
     </row>
     <row r="172">
       <c r="A172" t="n">
-        <v>171</v>
+        <v>865</v>
       </c>
       <c r="B172" t="n">
         <v>524</v>
@@ -4913,7 +4913,7 @@
     </row>
     <row r="173">
       <c r="A173" t="n">
-        <v>172</v>
+        <v>866</v>
       </c>
       <c r="B173" t="n">
         <v>1</v>
@@ -4939,7 +4939,7 @@
     </row>
     <row r="174">
       <c r="A174" t="n">
-        <v>173</v>
+        <v>867</v>
       </c>
       <c r="B174" t="n">
         <v>413</v>
@@ -4965,7 +4965,7 @@
     </row>
     <row r="175">
       <c r="A175" t="n">
-        <v>174</v>
+        <v>868</v>
       </c>
       <c r="B175" t="n">
         <v>414</v>
@@ -4991,7 +4991,7 @@
     </row>
     <row r="176">
       <c r="A176" t="n">
-        <v>175</v>
+        <v>869</v>
       </c>
       <c r="B176" t="n">
         <v>415</v>
@@ -5017,7 +5017,7 @@
     </row>
     <row r="177">
       <c r="A177" t="n">
-        <v>176</v>
+        <v>870</v>
       </c>
       <c r="B177" t="n">
         <v>416</v>
@@ -5043,7 +5043,7 @@
     </row>
     <row r="178">
       <c r="A178" t="n">
-        <v>177</v>
+        <v>871</v>
       </c>
       <c r="B178" t="n">
         <v>417</v>
@@ -5069,7 +5069,7 @@
     </row>
     <row r="179">
       <c r="A179" t="n">
-        <v>178</v>
+        <v>872</v>
       </c>
       <c r="B179" t="n">
         <v>418</v>
@@ -5095,7 +5095,7 @@
     </row>
     <row r="180">
       <c r="A180" t="n">
-        <v>179</v>
+        <v>873</v>
       </c>
       <c r="B180" t="n">
         <v>419</v>
@@ -5121,7 +5121,7 @@
     </row>
     <row r="181">
       <c r="A181" t="n">
-        <v>180</v>
+        <v>874</v>
       </c>
       <c r="B181" t="n">
         <v>420</v>
@@ -5147,7 +5147,7 @@
     </row>
     <row r="182">
       <c r="A182" t="n">
-        <v>181</v>
+        <v>875</v>
       </c>
       <c r="B182" t="n">
         <v>421</v>
@@ -5173,7 +5173,7 @@
     </row>
     <row r="183">
       <c r="A183" t="n">
-        <v>182</v>
+        <v>876</v>
       </c>
       <c r="B183" t="n">
         <v>2</v>
@@ -5199,7 +5199,7 @@
     </row>
     <row r="184">
       <c r="A184" t="n">
-        <v>183</v>
+        <v>877</v>
       </c>
       <c r="B184" t="n">
         <v>31</v>
@@ -5220,12 +5220,12 @@
         </is>
       </c>
       <c r="F184" t="n">
-        <v>14095</v>
+        <v>14173</v>
       </c>
     </row>
     <row r="185">
       <c r="A185" t="n">
-        <v>184</v>
+        <v>878</v>
       </c>
       <c r="B185" t="n">
         <v>32</v>
@@ -5251,7 +5251,7 @@
     </row>
     <row r="186">
       <c r="A186" t="n">
-        <v>185</v>
+        <v>879</v>
       </c>
       <c r="B186" t="n">
         <v>33</v>
@@ -5277,7 +5277,7 @@
     </row>
     <row r="187">
       <c r="A187" t="n">
-        <v>186</v>
+        <v>880</v>
       </c>
       <c r="B187" t="n">
         <v>34</v>
@@ -5298,12 +5298,12 @@
         </is>
       </c>
       <c r="F187" t="n">
-        <v>8461</v>
+        <v>8557</v>
       </c>
     </row>
     <row r="188">
       <c r="A188" t="n">
-        <v>187</v>
+        <v>881</v>
       </c>
       <c r="B188" t="n">
         <v>35</v>
@@ -5324,12 +5324,12 @@
         </is>
       </c>
       <c r="F188" t="n">
-        <v>6673</v>
+        <v>6721</v>
       </c>
     </row>
     <row r="189">
       <c r="A189" t="n">
-        <v>188</v>
+        <v>882</v>
       </c>
       <c r="B189" t="n">
         <v>36</v>
@@ -5350,12 +5350,12 @@
         </is>
       </c>
       <c r="F189" t="n">
-        <v>13385</v>
+        <v>13565</v>
       </c>
     </row>
     <row r="190">
       <c r="A190" t="n">
-        <v>189</v>
+        <v>883</v>
       </c>
       <c r="B190" t="n">
         <v>37</v>
@@ -5376,12 +5376,12 @@
         </is>
       </c>
       <c r="F190" t="n">
-        <v>3409</v>
+        <v>3433</v>
       </c>
     </row>
     <row r="191">
       <c r="A191" t="n">
-        <v>190</v>
+        <v>884</v>
       </c>
       <c r="B191" t="n">
         <v>38</v>
@@ -5407,7 +5407,7 @@
     </row>
     <row r="192">
       <c r="A192" t="n">
-        <v>191</v>
+        <v>885</v>
       </c>
       <c r="B192" t="n">
         <v>41</v>
@@ -5428,12 +5428,12 @@
         </is>
       </c>
       <c r="F192" t="n">
-        <v>21326</v>
+        <v>21611</v>
       </c>
     </row>
     <row r="193">
       <c r="A193" t="n">
-        <v>192</v>
+        <v>886</v>
       </c>
       <c r="B193" t="n">
         <v>42</v>
@@ -5459,7 +5459,7 @@
     </row>
     <row r="194">
       <c r="A194" t="n">
-        <v>193</v>
+        <v>887</v>
       </c>
       <c r="B194" t="n">
         <v>43</v>
@@ -5485,7 +5485,7 @@
     </row>
     <row r="195">
       <c r="A195" t="n">
-        <v>194</v>
+        <v>888</v>
       </c>
       <c r="B195" t="n">
         <v>44</v>
@@ -5506,12 +5506,12 @@
         </is>
       </c>
       <c r="F195" t="n">
-        <v>333</v>
+        <v>336</v>
       </c>
     </row>
     <row r="196">
       <c r="A196" t="n">
-        <v>195</v>
+        <v>889</v>
       </c>
       <c r="B196" t="n">
         <v>45</v>
@@ -5532,12 +5532,12 @@
         </is>
       </c>
       <c r="F196" t="n">
-        <v>743</v>
+        <v>749</v>
       </c>
     </row>
     <row r="197">
       <c r="A197" t="n">
-        <v>196</v>
+        <v>890</v>
       </c>
       <c r="B197" t="n">
         <v>46</v>
@@ -5558,12 +5558,12 @@
         </is>
       </c>
       <c r="F197" t="n">
-        <v>787</v>
+        <v>802</v>
       </c>
     </row>
     <row r="198">
       <c r="A198" t="n">
-        <v>197</v>
+        <v>891</v>
       </c>
       <c r="B198" t="n">
         <v>47</v>
@@ -5589,7 +5589,7 @@
     </row>
     <row r="199">
       <c r="A199" t="n">
-        <v>198</v>
+        <v>892</v>
       </c>
       <c r="B199" t="n">
         <v>48</v>
@@ -5610,12 +5610,12 @@
         </is>
       </c>
       <c r="F199" t="n">
-        <v>1698</v>
+        <v>1728</v>
       </c>
     </row>
     <row r="200">
       <c r="A200" t="n">
-        <v>199</v>
+        <v>893</v>
       </c>
       <c r="B200" t="n">
         <v>49</v>
@@ -5636,12 +5636,12 @@
         </is>
       </c>
       <c r="F200" t="n">
-        <v>5911</v>
+        <v>6010</v>
       </c>
     </row>
     <row r="201">
       <c r="A201" t="n">
-        <v>200</v>
+        <v>894</v>
       </c>
       <c r="B201" t="n">
         <v>410</v>
@@ -5662,12 +5662,12 @@
         </is>
       </c>
       <c r="F201" t="n">
-        <v>1486</v>
+        <v>1516</v>
       </c>
     </row>
     <row r="202">
       <c r="A202" t="n">
-        <v>201</v>
+        <v>895</v>
       </c>
       <c r="B202" t="n">
         <v>411</v>
@@ -5688,12 +5688,12 @@
         </is>
       </c>
       <c r="F202" t="n">
-        <v>1566</v>
+        <v>1593</v>
       </c>
     </row>
     <row r="203">
       <c r="A203" t="n">
-        <v>202</v>
+        <v>896</v>
       </c>
       <c r="B203" t="n">
         <v>412</v>
@@ -5714,12 +5714,12 @@
         </is>
       </c>
       <c r="F203" t="n">
-        <v>1666</v>
+        <v>1708</v>
       </c>
     </row>
     <row r="204">
       <c r="A204" t="n">
-        <v>203</v>
+        <v>897</v>
       </c>
       <c r="B204" t="n">
         <v>51</v>
@@ -5740,12 +5740,12 @@
         </is>
       </c>
       <c r="F204" t="n">
-        <v>2273</v>
+        <v>2348</v>
       </c>
     </row>
     <row r="205">
       <c r="A205" t="n">
-        <v>204</v>
+        <v>898</v>
       </c>
       <c r="B205" t="n">
         <v>52</v>
@@ -5766,12 +5766,12 @@
         </is>
       </c>
       <c r="F205" t="n">
-        <v>3190</v>
+        <v>3262</v>
       </c>
     </row>
     <row r="206">
       <c r="A206" t="n">
-        <v>205</v>
+        <v>899</v>
       </c>
       <c r="B206" t="n">
         <v>53</v>
@@ -5792,12 +5792,12 @@
         </is>
       </c>
       <c r="F206" t="n">
-        <v>11024</v>
+        <v>11237</v>
       </c>
     </row>
     <row r="207">
       <c r="A207" t="n">
-        <v>206</v>
+        <v>900</v>
       </c>
       <c r="B207" t="n">
         <v>54</v>
@@ -5818,12 +5818,12 @@
         </is>
       </c>
       <c r="F207" t="n">
-        <v>4360</v>
+        <v>4432</v>
       </c>
     </row>
     <row r="208">
       <c r="A208" t="n">
-        <v>207</v>
+        <v>901</v>
       </c>
       <c r="B208" t="n">
         <v>55</v>
@@ -5849,7 +5849,7 @@
     </row>
     <row r="209">
       <c r="A209" t="n">
-        <v>208</v>
+        <v>902</v>
       </c>
       <c r="B209" t="n">
         <v>56</v>
@@ -5875,7 +5875,7 @@
     </row>
     <row r="210">
       <c r="A210" t="n">
-        <v>209</v>
+        <v>903</v>
       </c>
       <c r="B210" t="n">
         <v>57</v>
@@ -5896,12 +5896,12 @@
         </is>
       </c>
       <c r="F210" t="n">
-        <v>1737</v>
+        <v>1758</v>
       </c>
     </row>
     <row r="211">
       <c r="A211" t="n">
-        <v>210</v>
+        <v>904</v>
       </c>
       <c r="B211" t="n">
         <v>58</v>
@@ -5922,12 +5922,12 @@
         </is>
       </c>
       <c r="F211" t="n">
-        <v>5817</v>
+        <v>5916</v>
       </c>
     </row>
     <row r="212">
       <c r="A212" t="n">
-        <v>211</v>
+        <v>905</v>
       </c>
       <c r="B212" t="n">
         <v>59</v>
@@ -5948,12 +5948,12 @@
         </is>
       </c>
       <c r="F212" t="n">
-        <v>11762</v>
+        <v>11939</v>
       </c>
     </row>
     <row r="213">
       <c r="A213" t="n">
-        <v>212</v>
+        <v>906</v>
       </c>
       <c r="B213" t="n">
         <v>510</v>
@@ -5974,12 +5974,12 @@
         </is>
       </c>
       <c r="F213" t="n">
-        <v>1122</v>
+        <v>1137</v>
       </c>
     </row>
     <row r="214">
       <c r="A214" t="n">
-        <v>213</v>
+        <v>907</v>
       </c>
       <c r="B214" t="n">
         <v>511</v>
@@ -6000,12 +6000,12 @@
         </is>
       </c>
       <c r="F214" t="n">
-        <v>417</v>
+        <v>423</v>
       </c>
     </row>
     <row r="215">
       <c r="A215" t="n">
-        <v>214</v>
+        <v>908</v>
       </c>
       <c r="B215" t="n">
         <v>512</v>
@@ -6031,7 +6031,7 @@
     </row>
     <row r="216">
       <c r="A216" t="n">
-        <v>215</v>
+        <v>909</v>
       </c>
       <c r="B216" t="n">
         <v>513</v>
@@ -6057,7 +6057,7 @@
     </row>
     <row r="217">
       <c r="A217" t="n">
-        <v>216</v>
+        <v>910</v>
       </c>
       <c r="B217" t="n">
         <v>514</v>
@@ -6083,7 +6083,7 @@
     </row>
     <row r="218">
       <c r="A218" t="n">
-        <v>217</v>
+        <v>911</v>
       </c>
       <c r="B218" t="n">
         <v>515</v>
@@ -6109,7 +6109,7 @@
     </row>
     <row r="219">
       <c r="A219" t="n">
-        <v>218</v>
+        <v>912</v>
       </c>
       <c r="B219" t="n">
         <v>516</v>
@@ -6135,7 +6135,7 @@
     </row>
     <row r="220">
       <c r="A220" t="n">
-        <v>219</v>
+        <v>913</v>
       </c>
       <c r="B220" t="n">
         <v>517</v>
@@ -6161,7 +6161,7 @@
     </row>
     <row r="221">
       <c r="A221" t="n">
-        <v>220</v>
+        <v>914</v>
       </c>
       <c r="B221" t="n">
         <v>518</v>
@@ -6187,7 +6187,7 @@
     </row>
     <row r="222">
       <c r="A222" t="n">
-        <v>221</v>
+        <v>915</v>
       </c>
       <c r="B222" t="n">
         <v>519</v>
@@ -6213,7 +6213,7 @@
     </row>
     <row r="223">
       <c r="A223" t="n">
-        <v>222</v>
+        <v>916</v>
       </c>
       <c r="B223" t="n">
         <v>520</v>
@@ -6239,7 +6239,7 @@
     </row>
     <row r="224">
       <c r="A224" t="n">
-        <v>223</v>
+        <v>917</v>
       </c>
       <c r="B224" t="n">
         <v>521</v>
@@ -6265,7 +6265,7 @@
     </row>
     <row r="225">
       <c r="A225" t="n">
-        <v>224</v>
+        <v>918</v>
       </c>
       <c r="B225" t="n">
         <v>522</v>
@@ -6291,7 +6291,7 @@
     </row>
     <row r="226">
       <c r="A226" t="n">
-        <v>225</v>
+        <v>919</v>
       </c>
       <c r="B226" t="n">
         <v>523</v>
@@ -6317,7 +6317,7 @@
     </row>
     <row r="227">
       <c r="A227" t="n">
-        <v>226</v>
+        <v>920</v>
       </c>
       <c r="B227" t="n">
         <v>524</v>
@@ -6343,7 +6343,7 @@
     </row>
     <row r="228">
       <c r="A228" t="n">
-        <v>227</v>
+        <v>921</v>
       </c>
       <c r="B228" t="n">
         <v>1</v>
@@ -6369,7 +6369,7 @@
     </row>
     <row r="229">
       <c r="A229" t="n">
-        <v>228</v>
+        <v>922</v>
       </c>
       <c r="B229" t="n">
         <v>413</v>
@@ -6395,7 +6395,7 @@
     </row>
     <row r="230">
       <c r="A230" t="n">
-        <v>229</v>
+        <v>923</v>
       </c>
       <c r="B230" t="n">
         <v>414</v>
@@ -6421,7 +6421,7 @@
     </row>
     <row r="231">
       <c r="A231" t="n">
-        <v>230</v>
+        <v>924</v>
       </c>
       <c r="B231" t="n">
         <v>415</v>
@@ -6447,7 +6447,7 @@
     </row>
     <row r="232">
       <c r="A232" t="n">
-        <v>231</v>
+        <v>925</v>
       </c>
       <c r="B232" t="n">
         <v>416</v>
@@ -6473,7 +6473,7 @@
     </row>
     <row r="233">
       <c r="A233" t="n">
-        <v>232</v>
+        <v>926</v>
       </c>
       <c r="B233" t="n">
         <v>417</v>
@@ -6499,7 +6499,7 @@
     </row>
     <row r="234">
       <c r="A234" t="n">
-        <v>233</v>
+        <v>927</v>
       </c>
       <c r="B234" t="n">
         <v>418</v>
@@ -6525,7 +6525,7 @@
     </row>
     <row r="235">
       <c r="A235" t="n">
-        <v>234</v>
+        <v>928</v>
       </c>
       <c r="B235" t="n">
         <v>419</v>
@@ -6551,7 +6551,7 @@
     </row>
     <row r="236">
       <c r="A236" t="n">
-        <v>235</v>
+        <v>929</v>
       </c>
       <c r="B236" t="n">
         <v>420</v>
@@ -6577,7 +6577,7 @@
     </row>
     <row r="237">
       <c r="A237" t="n">
-        <v>236</v>
+        <v>930</v>
       </c>
       <c r="B237" t="n">
         <v>421</v>
@@ -6603,7 +6603,7 @@
     </row>
     <row r="238">
       <c r="A238" t="n">
-        <v>237</v>
+        <v>931</v>
       </c>
       <c r="B238" t="n">
         <v>2</v>
@@ -6629,7 +6629,7 @@
     </row>
     <row r="239">
       <c r="A239" t="n">
-        <v>238</v>
+        <v>932</v>
       </c>
       <c r="B239" t="n">
         <v>31</v>
@@ -6650,12 +6650,12 @@
         </is>
       </c>
       <c r="F239" t="n">
-        <v>3832</v>
+        <v>3874</v>
       </c>
     </row>
     <row r="240">
       <c r="A240" t="n">
-        <v>239</v>
+        <v>933</v>
       </c>
       <c r="B240" t="n">
         <v>32</v>
@@ -6676,12 +6676,12 @@
         </is>
       </c>
       <c r="F240" t="n">
-        <v>212</v>
+        <v>215</v>
       </c>
     </row>
     <row r="241">
       <c r="A241" t="n">
-        <v>240</v>
+        <v>934</v>
       </c>
       <c r="B241" t="n">
         <v>33</v>
@@ -6707,7 +6707,7 @@
     </row>
     <row r="242">
       <c r="A242" t="n">
-        <v>241</v>
+        <v>935</v>
       </c>
       <c r="B242" t="n">
         <v>34</v>
@@ -6728,12 +6728,12 @@
         </is>
       </c>
       <c r="F242" t="n">
-        <v>3885</v>
+        <v>3957</v>
       </c>
     </row>
     <row r="243">
       <c r="A243" t="n">
-        <v>242</v>
+        <v>936</v>
       </c>
       <c r="B243" t="n">
         <v>35</v>
@@ -6754,12 +6754,12 @@
         </is>
       </c>
       <c r="F243" t="n">
-        <v>2625</v>
+        <v>2649</v>
       </c>
     </row>
     <row r="244">
       <c r="A244" t="n">
-        <v>243</v>
+        <v>937</v>
       </c>
       <c r="B244" t="n">
         <v>36</v>
@@ -6780,12 +6780,12 @@
         </is>
       </c>
       <c r="F244" t="n">
-        <v>8368</v>
+        <v>8464</v>
       </c>
     </row>
     <row r="245">
       <c r="A245" t="n">
-        <v>244</v>
+        <v>938</v>
       </c>
       <c r="B245" t="n">
         <v>37</v>
@@ -6806,12 +6806,12 @@
         </is>
       </c>
       <c r="F245" t="n">
-        <v>855</v>
+        <v>876</v>
       </c>
     </row>
     <row r="246">
       <c r="A246" t="n">
-        <v>245</v>
+        <v>939</v>
       </c>
       <c r="B246" t="n">
         <v>38</v>
@@ -6837,7 +6837,7 @@
     </row>
     <row r="247">
       <c r="A247" t="n">
-        <v>246</v>
+        <v>940</v>
       </c>
       <c r="B247" t="n">
         <v>41</v>
@@ -6858,12 +6858,12 @@
         </is>
       </c>
       <c r="F247" t="n">
-        <v>10856</v>
+        <v>11015</v>
       </c>
     </row>
     <row r="248">
       <c r="A248" t="n">
-        <v>247</v>
+        <v>941</v>
       </c>
       <c r="B248" t="n">
         <v>42</v>
@@ -6889,7 +6889,7 @@
     </row>
     <row r="249">
       <c r="A249" t="n">
-        <v>248</v>
+        <v>942</v>
       </c>
       <c r="B249" t="n">
         <v>43</v>
@@ -6915,7 +6915,7 @@
     </row>
     <row r="250">
       <c r="A250" t="n">
-        <v>249</v>
+        <v>943</v>
       </c>
       <c r="B250" t="n">
         <v>44</v>
@@ -6941,7 +6941,7 @@
     </row>
     <row r="251">
       <c r="A251" t="n">
-        <v>250</v>
+        <v>944</v>
       </c>
       <c r="B251" t="n">
         <v>45</v>
@@ -6962,12 +6962,12 @@
         </is>
       </c>
       <c r="F251" t="n">
-        <v>359</v>
+        <v>362</v>
       </c>
     </row>
     <row r="252">
       <c r="A252" t="n">
-        <v>251</v>
+        <v>945</v>
       </c>
       <c r="B252" t="n">
         <v>46</v>
@@ -6993,7 +6993,7 @@
     </row>
     <row r="253">
       <c r="A253" t="n">
-        <v>252</v>
+        <v>946</v>
       </c>
       <c r="B253" t="n">
         <v>47</v>
@@ -7019,7 +7019,7 @@
     </row>
     <row r="254">
       <c r="A254" t="n">
-        <v>253</v>
+        <v>947</v>
       </c>
       <c r="B254" t="n">
         <v>48</v>
@@ -7040,12 +7040,12 @@
         </is>
       </c>
       <c r="F254" t="n">
-        <v>478</v>
+        <v>487</v>
       </c>
     </row>
     <row r="255">
       <c r="A255" t="n">
-        <v>254</v>
+        <v>948</v>
       </c>
       <c r="B255" t="n">
         <v>49</v>
@@ -7066,12 +7066,12 @@
         </is>
       </c>
       <c r="F255" t="n">
-        <v>2950</v>
+        <v>2983</v>
       </c>
     </row>
     <row r="256">
       <c r="A256" t="n">
-        <v>255</v>
+        <v>949</v>
       </c>
       <c r="B256" t="n">
         <v>410</v>
@@ -7092,12 +7092,12 @@
         </is>
       </c>
       <c r="F256" t="n">
-        <v>527</v>
+        <v>542</v>
       </c>
     </row>
     <row r="257">
       <c r="A257" t="n">
-        <v>256</v>
+        <v>950</v>
       </c>
       <c r="B257" t="n">
         <v>411</v>
@@ -7118,12 +7118,12 @@
         </is>
       </c>
       <c r="F257" t="n">
-        <v>917</v>
+        <v>932</v>
       </c>
     </row>
     <row r="258">
       <c r="A258" t="n">
-        <v>257</v>
+        <v>951</v>
       </c>
       <c r="B258" t="n">
         <v>412</v>
@@ -7144,12 +7144,12 @@
         </is>
       </c>
       <c r="F258" t="n">
-        <v>570</v>
+        <v>597</v>
       </c>
     </row>
     <row r="259">
       <c r="A259" t="n">
-        <v>258</v>
+        <v>952</v>
       </c>
       <c r="B259" t="n">
         <v>51</v>
@@ -7170,12 +7170,12 @@
         </is>
       </c>
       <c r="F259" t="n">
-        <v>2455</v>
+        <v>2536</v>
       </c>
     </row>
     <row r="260">
       <c r="A260" t="n">
-        <v>259</v>
+        <v>953</v>
       </c>
       <c r="B260" t="n">
         <v>52</v>
@@ -7196,12 +7196,12 @@
         </is>
       </c>
       <c r="F260" t="n">
-        <v>1301</v>
+        <v>1328</v>
       </c>
     </row>
     <row r="261">
       <c r="A261" t="n">
-        <v>260</v>
+        <v>954</v>
       </c>
       <c r="B261" t="n">
         <v>53</v>
@@ -7222,12 +7222,12 @@
         </is>
       </c>
       <c r="F261" t="n">
-        <v>5597</v>
+        <v>5666</v>
       </c>
     </row>
     <row r="262">
       <c r="A262" t="n">
-        <v>261</v>
+        <v>955</v>
       </c>
       <c r="B262" t="n">
         <v>54</v>
@@ -7248,12 +7248,12 @@
         </is>
       </c>
       <c r="F262" t="n">
-        <v>3863</v>
+        <v>3941</v>
       </c>
     </row>
     <row r="263">
       <c r="A263" t="n">
-        <v>262</v>
+        <v>956</v>
       </c>
       <c r="B263" t="n">
         <v>55</v>
@@ -7274,12 +7274,12 @@
         </is>
       </c>
       <c r="F263" t="n">
-        <v>174</v>
+        <v>177</v>
       </c>
     </row>
     <row r="264">
       <c r="A264" t="n">
-        <v>263</v>
+        <v>957</v>
       </c>
       <c r="B264" t="n">
         <v>56</v>
@@ -7305,7 +7305,7 @@
     </row>
     <row r="265">
       <c r="A265" t="n">
-        <v>264</v>
+        <v>958</v>
       </c>
       <c r="B265" t="n">
         <v>57</v>
@@ -7326,12 +7326,12 @@
         </is>
       </c>
       <c r="F265" t="n">
-        <v>883</v>
+        <v>889</v>
       </c>
     </row>
     <row r="266">
       <c r="A266" t="n">
-        <v>265</v>
+        <v>959</v>
       </c>
       <c r="B266" t="n">
         <v>58</v>
@@ -7352,12 +7352,12 @@
         </is>
       </c>
       <c r="F266" t="n">
-        <v>3224</v>
+        <v>3278</v>
       </c>
     </row>
     <row r="267">
       <c r="A267" t="n">
-        <v>266</v>
+        <v>960</v>
       </c>
       <c r="B267" t="n">
         <v>59</v>
@@ -7378,12 +7378,12 @@
         </is>
       </c>
       <c r="F267" t="n">
-        <v>7066</v>
+        <v>7150</v>
       </c>
     </row>
     <row r="268">
       <c r="A268" t="n">
-        <v>267</v>
+        <v>961</v>
       </c>
       <c r="B268" t="n">
         <v>510</v>
@@ -7404,12 +7404,12 @@
         </is>
       </c>
       <c r="F268" t="n">
-        <v>943</v>
+        <v>958</v>
       </c>
     </row>
     <row r="269">
       <c r="A269" t="n">
-        <v>268</v>
+        <v>962</v>
       </c>
       <c r="B269" t="n">
         <v>511</v>
@@ -7435,7 +7435,7 @@
     </row>
     <row r="270">
       <c r="A270" t="n">
-        <v>269</v>
+        <v>963</v>
       </c>
       <c r="B270" t="n">
         <v>512</v>
@@ -7461,7 +7461,7 @@
     </row>
     <row r="271">
       <c r="A271" t="n">
-        <v>270</v>
+        <v>964</v>
       </c>
       <c r="B271" t="n">
         <v>513</v>
@@ -7487,7 +7487,7 @@
     </row>
     <row r="272">
       <c r="A272" t="n">
-        <v>271</v>
+        <v>965</v>
       </c>
       <c r="B272" t="n">
         <v>514</v>
@@ -7513,7 +7513,7 @@
     </row>
     <row r="273">
       <c r="A273" t="n">
-        <v>272</v>
+        <v>966</v>
       </c>
       <c r="B273" t="n">
         <v>515</v>
@@ -7539,7 +7539,7 @@
     </row>
     <row r="274">
       <c r="A274" t="n">
-        <v>273</v>
+        <v>967</v>
       </c>
       <c r="B274" t="n">
         <v>516</v>
@@ -7565,7 +7565,7 @@
     </row>
     <row r="275">
       <c r="A275" t="n">
-        <v>274</v>
+        <v>968</v>
       </c>
       <c r="B275" t="n">
         <v>517</v>
@@ -7591,7 +7591,7 @@
     </row>
     <row r="276">
       <c r="A276" t="n">
-        <v>275</v>
+        <v>969</v>
       </c>
       <c r="B276" t="n">
         <v>518</v>
@@ -7617,7 +7617,7 @@
     </row>
     <row r="277">
       <c r="A277" t="n">
-        <v>276</v>
+        <v>970</v>
       </c>
       <c r="B277" t="n">
         <v>519</v>
@@ -7643,7 +7643,7 @@
     </row>
     <row r="278">
       <c r="A278" t="n">
-        <v>277</v>
+        <v>971</v>
       </c>
       <c r="B278" t="n">
         <v>520</v>
@@ -7669,7 +7669,7 @@
     </row>
     <row r="279">
       <c r="A279" t="n">
-        <v>278</v>
+        <v>972</v>
       </c>
       <c r="B279" t="n">
         <v>521</v>
@@ -7695,7 +7695,7 @@
     </row>
     <row r="280">
       <c r="A280" t="n">
-        <v>279</v>
+        <v>973</v>
       </c>
       <c r="B280" t="n">
         <v>522</v>
@@ -7721,7 +7721,7 @@
     </row>
     <row r="281">
       <c r="A281" t="n">
-        <v>280</v>
+        <v>974</v>
       </c>
       <c r="B281" t="n">
         <v>523</v>
@@ -7747,7 +7747,7 @@
     </row>
     <row r="282">
       <c r="A282" t="n">
-        <v>281</v>
+        <v>975</v>
       </c>
       <c r="B282" t="n">
         <v>524</v>
@@ -7773,7 +7773,7 @@
     </row>
     <row r="283">
       <c r="A283" t="n">
-        <v>282</v>
+        <v>976</v>
       </c>
       <c r="B283" t="n">
         <v>1</v>
@@ -7799,7 +7799,7 @@
     </row>
     <row r="284">
       <c r="A284" t="n">
-        <v>283</v>
+        <v>977</v>
       </c>
       <c r="B284" t="n">
         <v>413</v>
@@ -7825,7 +7825,7 @@
     </row>
     <row r="285">
       <c r="A285" t="n">
-        <v>284</v>
+        <v>978</v>
       </c>
       <c r="B285" t="n">
         <v>414</v>
@@ -7851,7 +7851,7 @@
     </row>
     <row r="286">
       <c r="A286" t="n">
-        <v>285</v>
+        <v>979</v>
       </c>
       <c r="B286" t="n">
         <v>415</v>
@@ -7877,7 +7877,7 @@
     </row>
     <row r="287">
       <c r="A287" t="n">
-        <v>286</v>
+        <v>980</v>
       </c>
       <c r="B287" t="n">
         <v>416</v>
@@ -7903,7 +7903,7 @@
     </row>
     <row r="288">
       <c r="A288" t="n">
-        <v>287</v>
+        <v>981</v>
       </c>
       <c r="B288" t="n">
         <v>417</v>
@@ -7929,7 +7929,7 @@
     </row>
     <row r="289">
       <c r="A289" t="n">
-        <v>288</v>
+        <v>982</v>
       </c>
       <c r="B289" t="n">
         <v>418</v>
@@ -7955,7 +7955,7 @@
     </row>
     <row r="290">
       <c r="A290" t="n">
-        <v>289</v>
+        <v>983</v>
       </c>
       <c r="B290" t="n">
         <v>419</v>
@@ -7981,7 +7981,7 @@
     </row>
     <row r="291">
       <c r="A291" t="n">
-        <v>290</v>
+        <v>984</v>
       </c>
       <c r="B291" t="n">
         <v>420</v>
@@ -8007,7 +8007,7 @@
     </row>
     <row r="292">
       <c r="A292" t="n">
-        <v>291</v>
+        <v>985</v>
       </c>
       <c r="B292" t="n">
         <v>421</v>
@@ -8033,7 +8033,7 @@
     </row>
     <row r="293">
       <c r="A293" t="n">
-        <v>292</v>
+        <v>986</v>
       </c>
       <c r="B293" t="n">
         <v>2</v>
@@ -8059,7 +8059,7 @@
     </row>
     <row r="294">
       <c r="A294" t="n">
-        <v>293</v>
+        <v>987</v>
       </c>
       <c r="B294" t="n">
         <v>31</v>
@@ -8080,12 +8080,12 @@
         </is>
       </c>
       <c r="F294" t="n">
-        <v>4617</v>
+        <v>4638</v>
       </c>
     </row>
     <row r="295">
       <c r="A295" t="n">
-        <v>294</v>
+        <v>988</v>
       </c>
       <c r="B295" t="n">
         <v>32</v>
@@ -8111,7 +8111,7 @@
     </row>
     <row r="296">
       <c r="A296" t="n">
-        <v>295</v>
+        <v>989</v>
       </c>
       <c r="B296" t="n">
         <v>33</v>
@@ -8137,7 +8137,7 @@
     </row>
     <row r="297">
       <c r="A297" t="n">
-        <v>296</v>
+        <v>990</v>
       </c>
       <c r="B297" t="n">
         <v>34</v>
@@ -8158,12 +8158,12 @@
         </is>
       </c>
       <c r="F297" t="n">
-        <v>3593</v>
+        <v>3635</v>
       </c>
     </row>
     <row r="298">
       <c r="A298" t="n">
-        <v>297</v>
+        <v>991</v>
       </c>
       <c r="B298" t="n">
         <v>35</v>
@@ -8184,12 +8184,12 @@
         </is>
       </c>
       <c r="F298" t="n">
-        <v>2333</v>
+        <v>2357</v>
       </c>
     </row>
     <row r="299">
       <c r="A299" t="n">
-        <v>298</v>
+        <v>992</v>
       </c>
       <c r="B299" t="n">
         <v>36</v>
@@ -8210,12 +8210,12 @@
         </is>
       </c>
       <c r="F299" t="n">
-        <v>8039</v>
+        <v>8114</v>
       </c>
     </row>
     <row r="300">
       <c r="A300" t="n">
-        <v>299</v>
+        <v>993</v>
       </c>
       <c r="B300" t="n">
         <v>37</v>
@@ -8236,12 +8236,12 @@
         </is>
       </c>
       <c r="F300" t="n">
-        <v>964</v>
+        <v>982</v>
       </c>
     </row>
     <row r="301">
       <c r="A301" t="n">
-        <v>300</v>
+        <v>994</v>
       </c>
       <c r="B301" t="n">
         <v>38</v>
@@ -8267,7 +8267,7 @@
     </row>
     <row r="302">
       <c r="A302" t="n">
-        <v>301</v>
+        <v>995</v>
       </c>
       <c r="B302" t="n">
         <v>41</v>
@@ -8288,12 +8288,12 @@
         </is>
       </c>
       <c r="F302" t="n">
-        <v>11047</v>
+        <v>11224</v>
       </c>
     </row>
     <row r="303">
       <c r="A303" t="n">
-        <v>302</v>
+        <v>996</v>
       </c>
       <c r="B303" t="n">
         <v>42</v>
@@ -8319,7 +8319,7 @@
     </row>
     <row r="304">
       <c r="A304" t="n">
-        <v>303</v>
+        <v>997</v>
       </c>
       <c r="B304" t="n">
         <v>43</v>
@@ -8345,7 +8345,7 @@
     </row>
     <row r="305">
       <c r="A305" t="n">
-        <v>304</v>
+        <v>998</v>
       </c>
       <c r="B305" t="n">
         <v>44</v>
@@ -8371,7 +8371,7 @@
     </row>
     <row r="306">
       <c r="A306" t="n">
-        <v>305</v>
+        <v>999</v>
       </c>
       <c r="B306" t="n">
         <v>45</v>
@@ -8392,12 +8392,12 @@
         </is>
       </c>
       <c r="F306" t="n">
-        <v>227</v>
+        <v>233</v>
       </c>
     </row>
     <row r="307">
       <c r="A307" t="n">
-        <v>306</v>
+        <v>1000</v>
       </c>
       <c r="B307" t="n">
         <v>46</v>
@@ -8423,7 +8423,7 @@
     </row>
     <row r="308">
       <c r="A308" t="n">
-        <v>307</v>
+        <v>1001</v>
       </c>
       <c r="B308" t="n">
         <v>47</v>
@@ -8444,12 +8444,12 @@
         </is>
       </c>
       <c r="F308" t="n">
-        <v>92</v>
+        <v>95</v>
       </c>
     </row>
     <row r="309">
       <c r="A309" t="n">
-        <v>308</v>
+        <v>1002</v>
       </c>
       <c r="B309" t="n">
         <v>48</v>
@@ -8470,12 +8470,12 @@
         </is>
       </c>
       <c r="F309" t="n">
-        <v>520</v>
+        <v>526</v>
       </c>
     </row>
     <row r="310">
       <c r="A310" t="n">
-        <v>309</v>
+        <v>1003</v>
       </c>
       <c r="B310" t="n">
         <v>49</v>
@@ -8496,12 +8496,12 @@
         </is>
       </c>
       <c r="F310" t="n">
-        <v>3251</v>
+        <v>3299</v>
       </c>
     </row>
     <row r="311">
       <c r="A311" t="n">
-        <v>310</v>
+        <v>1004</v>
       </c>
       <c r="B311" t="n">
         <v>410</v>
@@ -8522,12 +8522,12 @@
         </is>
       </c>
       <c r="F311" t="n">
-        <v>705</v>
+        <v>717</v>
       </c>
     </row>
     <row r="312">
       <c r="A312" t="n">
-        <v>311</v>
+        <v>1005</v>
       </c>
       <c r="B312" t="n">
         <v>411</v>
@@ -8548,12 +8548,12 @@
         </is>
       </c>
       <c r="F312" t="n">
-        <v>870</v>
+        <v>882</v>
       </c>
     </row>
     <row r="313">
       <c r="A313" t="n">
-        <v>312</v>
+        <v>1006</v>
       </c>
       <c r="B313" t="n">
         <v>412</v>
@@ -8574,12 +8574,12 @@
         </is>
       </c>
       <c r="F313" t="n">
-        <v>559</v>
+        <v>571</v>
       </c>
     </row>
     <row r="314">
       <c r="A314" t="n">
-        <v>313</v>
+        <v>1007</v>
       </c>
       <c r="B314" t="n">
         <v>51</v>
@@ -8600,12 +8600,12 @@
         </is>
       </c>
       <c r="F314" t="n">
-        <v>1087</v>
+        <v>1126</v>
       </c>
     </row>
     <row r="315">
       <c r="A315" t="n">
-        <v>314</v>
+        <v>1008</v>
       </c>
       <c r="B315" t="n">
         <v>52</v>
@@ -8626,12 +8626,12 @@
         </is>
       </c>
       <c r="F315" t="n">
-        <v>1575</v>
+        <v>1605</v>
       </c>
     </row>
     <row r="316">
       <c r="A316" t="n">
-        <v>315</v>
+        <v>1009</v>
       </c>
       <c r="B316" t="n">
         <v>53</v>
@@ -8652,12 +8652,12 @@
         </is>
       </c>
       <c r="F316" t="n">
-        <v>5623</v>
+        <v>5737</v>
       </c>
     </row>
     <row r="317">
       <c r="A317" t="n">
-        <v>316</v>
+        <v>1010</v>
       </c>
       <c r="B317" t="n">
         <v>54</v>
@@ -8678,12 +8678,12 @@
         </is>
       </c>
       <c r="F317" t="n">
-        <v>1992</v>
+        <v>2034</v>
       </c>
     </row>
     <row r="318">
       <c r="A318" t="n">
-        <v>317</v>
+        <v>1011</v>
       </c>
       <c r="B318" t="n">
         <v>55</v>
@@ -8704,12 +8704,12 @@
         </is>
       </c>
       <c r="F318" t="n">
-        <v>208</v>
+        <v>211</v>
       </c>
     </row>
     <row r="319">
       <c r="A319" t="n">
-        <v>318</v>
+        <v>1012</v>
       </c>
       <c r="B319" t="n">
         <v>56</v>
@@ -8735,7 +8735,7 @@
     </row>
     <row r="320">
       <c r="A320" t="n">
-        <v>319</v>
+        <v>1013</v>
       </c>
       <c r="B320" t="n">
         <v>57</v>
@@ -8756,12 +8756,12 @@
         </is>
       </c>
       <c r="F320" t="n">
-        <v>833</v>
+        <v>836</v>
       </c>
     </row>
     <row r="321">
       <c r="A321" t="n">
-        <v>320</v>
+        <v>1014</v>
       </c>
       <c r="B321" t="n">
         <v>58</v>
@@ -8782,12 +8782,12 @@
         </is>
       </c>
       <c r="F321" t="n">
-        <v>2321</v>
+        <v>2339</v>
       </c>
     </row>
     <row r="322">
       <c r="A322" t="n">
-        <v>321</v>
+        <v>1015</v>
       </c>
       <c r="B322" t="n">
         <v>59</v>
@@ -8808,12 +8808,12 @@
         </is>
       </c>
       <c r="F322" t="n">
-        <v>7266</v>
+        <v>7353</v>
       </c>
     </row>
     <row r="323">
       <c r="A323" t="n">
-        <v>322</v>
+        <v>1016</v>
       </c>
       <c r="B323" t="n">
         <v>510</v>
@@ -8834,12 +8834,12 @@
         </is>
       </c>
       <c r="F323" t="n">
-        <v>831</v>
+        <v>843</v>
       </c>
     </row>
     <row r="324">
       <c r="A324" t="n">
-        <v>323</v>
+        <v>1017</v>
       </c>
       <c r="B324" t="n">
         <v>511</v>
@@ -8865,7 +8865,7 @@
     </row>
     <row r="325">
       <c r="A325" t="n">
-        <v>324</v>
+        <v>1018</v>
       </c>
       <c r="B325" t="n">
         <v>512</v>
@@ -8891,7 +8891,7 @@
     </row>
     <row r="326">
       <c r="A326" t="n">
-        <v>325</v>
+        <v>1019</v>
       </c>
       <c r="B326" t="n">
         <v>513</v>
@@ -8917,7 +8917,7 @@
     </row>
     <row r="327">
       <c r="A327" t="n">
-        <v>326</v>
+        <v>1020</v>
       </c>
       <c r="B327" t="n">
         <v>514</v>
@@ -8943,7 +8943,7 @@
     </row>
     <row r="328">
       <c r="A328" t="n">
-        <v>327</v>
+        <v>1021</v>
       </c>
       <c r="B328" t="n">
         <v>515</v>
@@ -8969,7 +8969,7 @@
     </row>
     <row r="329">
       <c r="A329" t="n">
-        <v>328</v>
+        <v>1022</v>
       </c>
       <c r="B329" t="n">
         <v>516</v>
@@ -8995,7 +8995,7 @@
     </row>
     <row r="330">
       <c r="A330" t="n">
-        <v>329</v>
+        <v>1023</v>
       </c>
       <c r="B330" t="n">
         <v>517</v>
@@ -9021,7 +9021,7 @@
     </row>
     <row r="331">
       <c r="A331" t="n">
-        <v>330</v>
+        <v>1024</v>
       </c>
       <c r="B331" t="n">
         <v>518</v>
@@ -9047,7 +9047,7 @@
     </row>
     <row r="332">
       <c r="A332" t="n">
-        <v>331</v>
+        <v>1025</v>
       </c>
       <c r="B332" t="n">
         <v>519</v>
@@ -9073,7 +9073,7 @@
     </row>
     <row r="333">
       <c r="A333" t="n">
-        <v>332</v>
+        <v>1026</v>
       </c>
       <c r="B333" t="n">
         <v>520</v>
@@ -9099,7 +9099,7 @@
     </row>
     <row r="334">
       <c r="A334" t="n">
-        <v>333</v>
+        <v>1027</v>
       </c>
       <c r="B334" t="n">
         <v>521</v>
@@ -9125,7 +9125,7 @@
     </row>
     <row r="335">
       <c r="A335" t="n">
-        <v>334</v>
+        <v>1028</v>
       </c>
       <c r="B335" t="n">
         <v>522</v>
@@ -9151,7 +9151,7 @@
     </row>
     <row r="336">
       <c r="A336" t="n">
-        <v>335</v>
+        <v>1029</v>
       </c>
       <c r="B336" t="n">
         <v>523</v>
@@ -9177,7 +9177,7 @@
     </row>
     <row r="337">
       <c r="A337" t="n">
-        <v>336</v>
+        <v>1030</v>
       </c>
       <c r="B337" t="n">
         <v>524</v>
@@ -9203,7 +9203,7 @@
     </row>
     <row r="338">
       <c r="A338" t="n">
-        <v>337</v>
+        <v>1031</v>
       </c>
       <c r="B338" t="n">
         <v>1</v>
@@ -9229,7 +9229,7 @@
     </row>
     <row r="339">
       <c r="A339" t="n">
-        <v>338</v>
+        <v>1032</v>
       </c>
       <c r="B339" t="n">
         <v>413</v>
@@ -9255,7 +9255,7 @@
     </row>
     <row r="340">
       <c r="A340" t="n">
-        <v>339</v>
+        <v>1033</v>
       </c>
       <c r="B340" t="n">
         <v>414</v>
@@ -9281,7 +9281,7 @@
     </row>
     <row r="341">
       <c r="A341" t="n">
-        <v>340</v>
+        <v>1034</v>
       </c>
       <c r="B341" t="n">
         <v>415</v>
@@ -9307,7 +9307,7 @@
     </row>
     <row r="342">
       <c r="A342" t="n">
-        <v>341</v>
+        <v>1035</v>
       </c>
       <c r="B342" t="n">
         <v>416</v>
@@ -9333,7 +9333,7 @@
     </row>
     <row r="343">
       <c r="A343" t="n">
-        <v>342</v>
+        <v>1036</v>
       </c>
       <c r="B343" t="n">
         <v>417</v>
@@ -9359,7 +9359,7 @@
     </row>
     <row r="344">
       <c r="A344" t="n">
-        <v>343</v>
+        <v>1037</v>
       </c>
       <c r="B344" t="n">
         <v>418</v>
@@ -9385,7 +9385,7 @@
     </row>
     <row r="345">
       <c r="A345" t="n">
-        <v>344</v>
+        <v>1038</v>
       </c>
       <c r="B345" t="n">
         <v>419</v>
@@ -9411,7 +9411,7 @@
     </row>
     <row r="346">
       <c r="A346" t="n">
-        <v>345</v>
+        <v>1039</v>
       </c>
       <c r="B346" t="n">
         <v>420</v>
@@ -9437,7 +9437,7 @@
     </row>
     <row r="347">
       <c r="A347" t="n">
-        <v>346</v>
+        <v>1040</v>
       </c>
       <c r="B347" t="n">
         <v>421</v>
@@ -9463,7 +9463,7 @@
     </row>
     <row r="348">
       <c r="A348" t="n">
-        <v>347</v>
+        <v>1041</v>
       </c>
       <c r="B348" t="n">
         <v>2</v>

</xml_diff>